<commit_message>
Fixed error with offtopic article 17 by 18
</commit_message>
<xml_diff>
--- a/joined_recs_freeze_march.xlsx
+++ b/joined_recs_freeze_march.xlsx
@@ -2060,6 +2060,9 @@
     <t>Soft Comput.</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>India</t>
   </si>
   <si>
@@ -2160,9 +2163,6 @@
   </si>
   <si>
     <t>Internet Things</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>10.1016/j.iot.2021.100461</t>
@@ -8783,25 +8783,25 @@
         <v>678</v>
       </c>
       <c r="BF17" s="4" t="s">
-        <v>145</v>
+        <v>679</v>
       </c>
       <c r="BG17" s="4" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="BH17" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="BI17" s="3">
         <v>0.0</v>
       </c>
       <c r="BK17" s="3" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="BL17" s="3">
         <v>22.0</v>
       </c>
       <c r="BM17" s="3" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="BN17" s="3" t="s">
         <v>149</v>
@@ -8810,22 +8810,22 @@
         <v>242</v>
       </c>
       <c r="BP17" s="3" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="BU17" s="3" t="s">
         <v>152</v>
       </c>
       <c r="BV17" s="3" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="BW17" s="3">
         <v>0.0</v>
       </c>
       <c r="BX17" s="3" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="BY17" s="3" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="BZ17" s="3" t="s">
         <v>664</v>
@@ -8834,37 +8834,37 @@
         <v>2021.0</v>
       </c>
       <c r="CB17" s="3" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="CJ17" s="3" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="CK17" s="3" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="CL17" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CM17" s="3" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="CN17" s="3" t="s">
         <v>667</v>
       </c>
       <c r="CO17" s="3" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="CW17" s="3" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="CX17" s="3" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="DA17" s="3" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="DF17" s="3" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="DJ17" s="3" t="s">
         <v>125</v>
@@ -8876,13 +8876,13 @@
         <v>126</v>
       </c>
       <c r="DM17" s="3" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="DO17" s="3" t="s">
         <v>172</v>
       </c>
       <c r="DP17" s="3" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="DQ17" s="3" t="s">
         <v>174</v>
@@ -8896,16 +8896,16 @@
         <v>120</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>125</v>
@@ -8914,22 +8914,22 @@
         <v>126</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="V18" s="3" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="AA18" s="3" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="AH18" s="3">
         <v>106.0</v>
@@ -8956,16 +8956,16 @@
         <v>371</v>
       </c>
       <c r="AP18" s="3" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AQ18" s="3" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="AS18" s="3" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="AT18" s="3" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="AU18" s="3" t="s">
         <v>193</v>
@@ -8980,10 +8980,10 @@
         <v>100461.0</v>
       </c>
       <c r="BF18" s="4" t="s">
-        <v>713</v>
+        <v>145</v>
       </c>
       <c r="BG18" s="4" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="BH18" s="3" t="s">
         <v>714</v>
@@ -10251,7 +10251,7 @@
         <v>145</v>
       </c>
       <c r="BG25" s="4" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="BH25" s="3" t="s">
         <v>892</v>
@@ -10314,7 +10314,7 @@
         <v>906</v>
       </c>
       <c r="DA25" s="3" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="DF25" s="3" t="s">
         <v>907</v>
@@ -10346,7 +10346,7 @@
         <v>34.0</v>
       </c>
       <c r="BF26" s="4" t="s">
-        <v>713</v>
+        <v>679</v>
       </c>
       <c r="BG26" s="4" t="s">
         <v>146</v>
@@ -10507,7 +10507,7 @@
         <v>126</v>
       </c>
       <c r="DM27" s="3" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="DO27" s="3" t="s">
         <v>172</v>
@@ -10622,7 +10622,7 @@
         <v>38.0</v>
       </c>
       <c r="BF29" s="4" t="s">
-        <v>713</v>
+        <v>679</v>
       </c>
       <c r="BG29" s="4" t="s">
         <v>146</v>
@@ -12864,7 +12864,7 @@
         <v>62.0</v>
       </c>
       <c r="BF52" s="6" t="s">
-        <v>713</v>
+        <v>679</v>
       </c>
       <c r="BG52" s="4" t="s">
         <v>1303</v>
@@ -13057,7 +13057,7 @@
         <v>64.0</v>
       </c>
       <c r="BF54" s="4" t="s">
-        <v>713</v>
+        <v>679</v>
       </c>
       <c r="BG54" s="4" t="s">
         <v>146</v>
@@ -13515,7 +13515,7 @@
         <v>126</v>
       </c>
       <c r="DM58" s="3" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="DO58" s="3" t="s">
         <v>172</v>

</xml_diff>